<commit_message>
Rerun experiment for xdribble model only
</commit_message>
<xml_diff>
--- a/notebooks/data/players_skill_dataset/Transfermarkt Euro 2020 Comparison.xlsx
+++ b/notebooks/data/players_skill_dataset/Transfermarkt Euro 2020 Comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://itbdsti-my.sharepoint.com/personal/23522016_mahasiswa_itb_ac_id/Documents/Informatika S2/Semester 3/IF6099 Thesis/Draft Thesis/Thesis/Source Code/vaep-base-code/notebooks/data/players_skill_dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="572" documentId="11_F25DC773A252ABDACC104849C99C61665BDE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AF35EB6-1051-4BD7-BB9F-AB7EA8B30A92}"/>
+  <xr:revisionPtr revIDLastSave="605" documentId="11_F25DC773A252ABDACC104849C99C61665BDE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D13A325E-BD36-41B6-82CF-0FD0A2754DCE}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -261,6 +261,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -584,19 +588,19 @@
         <v>2</v>
       </c>
       <c r="E2">
-        <f>C2+D2</f>
+        <f t="shared" ref="E2:E19" si="0">C2+D2</f>
         <v>2</v>
       </c>
       <c r="F2">
-        <f xml:space="preserve"> (90 / B2) * C2</f>
+        <f t="shared" ref="F2:F19" si="1" xml:space="preserve"> (90 / B2) * C2</f>
         <v>0</v>
       </c>
       <c r="G2">
-        <f>(90/B2)*D2</f>
+        <f t="shared" ref="G2:G19" si="2">(90/B2)*D2</f>
         <v>4.3902439024390247</v>
       </c>
       <c r="H2">
-        <f>(90/B2) * E2</f>
+        <f t="shared" ref="H2:H19" si="3">(90/B2) * E2</f>
         <v>4.3902439024390247</v>
       </c>
     </row>
@@ -614,19 +618,19 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <f>C3+D3</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F3">
-        <f xml:space="preserve"> (90 / B3) * C3</f>
+        <f t="shared" si="1"/>
         <v>0.74380165289256195</v>
       </c>
       <c r="G3">
-        <f>(90/B3)*D3</f>
+        <f t="shared" si="2"/>
         <v>0.74380165289256195</v>
       </c>
       <c r="H3">
-        <f>(90/B3) * E3</f>
+        <f t="shared" si="3"/>
         <v>1.4876033057851239</v>
       </c>
     </row>
@@ -644,19 +648,19 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <f>C4+D4</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F4">
-        <f xml:space="preserve"> (90 / B4) * C4</f>
+        <f t="shared" si="1"/>
         <v>1.267605633802817</v>
       </c>
       <c r="G4">
-        <f>(90/B4)*D4</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f>(90/B4) * E4</f>
+        <f t="shared" si="3"/>
         <v>1.267605633802817</v>
       </c>
     </row>
@@ -674,19 +678,19 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <f>C5+D5</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="F5">
-        <f xml:space="preserve"> (90 / B5) * C5</f>
+        <f t="shared" si="1"/>
         <v>0.66420664206642066</v>
       </c>
       <c r="G5">
-        <f>(90/B5)*D5</f>
+        <f t="shared" si="2"/>
         <v>0.33210332103321033</v>
       </c>
       <c r="H5">
-        <f>(90/B5) * E5</f>
+        <f t="shared" si="3"/>
         <v>0.99630996309963105</v>
       </c>
     </row>
@@ -704,19 +708,19 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <f>C6+D6</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="F6">
-        <f xml:space="preserve"> (90 / B6) * C6</f>
+        <f t="shared" si="1"/>
         <v>0.96256684491978606</v>
       </c>
       <c r="G6">
-        <f>(90/B6)*D6</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H6">
-        <f>(90/B6) * E6</f>
+        <f t="shared" si="3"/>
         <v>0.96256684491978606</v>
       </c>
     </row>
@@ -734,19 +738,19 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <f>C7+D7</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="F7">
-        <f xml:space="preserve"> (90 / B7) * C7</f>
+        <f t="shared" si="1"/>
         <v>0.87662337662337664</v>
       </c>
       <c r="G7">
-        <f>(90/B7)*D7</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H7">
-        <f>(90/B7) * E7</f>
+        <f t="shared" si="3"/>
         <v>0.87662337662337664</v>
       </c>
     </row>
@@ -764,19 +768,19 @@
         <v>2</v>
       </c>
       <c r="E8">
-        <f>C8+D8</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F8">
-        <f xml:space="preserve"> (90 / B8) * C8</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G8">
-        <f>(90/B8)*D8</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="H8">
-        <f>(90/B8) * E8</f>
+        <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
     </row>
@@ -794,19 +798,19 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <f>C9+D9</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F9">
-        <f xml:space="preserve"> (90 / B9) * C9</f>
+        <f t="shared" si="1"/>
         <v>0.69498069498069504</v>
       </c>
       <c r="G9">
-        <f>(90/B9)*D9</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H9">
-        <f>(90/B9) * E9</f>
+        <f t="shared" si="3"/>
         <v>0.69498069498069504</v>
       </c>
     </row>
@@ -824,19 +828,19 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <f>C10+D10</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="F10">
-        <f xml:space="preserve"> (90 / B10) * C10</f>
+        <f t="shared" si="1"/>
         <v>0.4580152671755725</v>
       </c>
       <c r="G10">
-        <f>(90/B10)*D10</f>
+        <f t="shared" si="2"/>
         <v>0.22900763358778625</v>
       </c>
       <c r="H10">
-        <f>(90/B10) * E10</f>
+        <f t="shared" si="3"/>
         <v>0.68702290076335881</v>
       </c>
     </row>
@@ -854,19 +858,19 @@
         <v>2</v>
       </c>
       <c r="E11">
-        <f>C11+D11</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F11">
-        <f xml:space="preserve"> (90 / B11) * C11</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G11">
-        <f>(90/B11)*D11</f>
+        <f t="shared" si="2"/>
         <v>0.62937062937062938</v>
       </c>
       <c r="H11">
-        <f>(90/B11) * E11</f>
+        <f t="shared" si="3"/>
         <v>0.62937062937062938</v>
       </c>
     </row>
@@ -884,19 +888,19 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <f>C12+D12</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F12">
-        <f xml:space="preserve"> (90 / B12) * C12</f>
+        <f t="shared" si="1"/>
         <v>0.29411764705882354</v>
       </c>
       <c r="G12">
-        <f>(90/B12)*D12</f>
+        <f t="shared" si="2"/>
         <v>0.29411764705882354</v>
       </c>
       <c r="H12">
-        <f>(90/B12) * E12</f>
+        <f t="shared" si="3"/>
         <v>0.58823529411764708</v>
       </c>
     </row>
@@ -914,19 +918,19 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <f>C13+D13</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F13">
-        <f xml:space="preserve"> (90 / B13) * C13</f>
+        <f t="shared" si="1"/>
         <v>0.28938906752411575</v>
       </c>
       <c r="G13">
-        <f>(90/B13)*D13</f>
+        <f t="shared" si="2"/>
         <v>0.28938906752411575</v>
       </c>
       <c r="H13">
-        <f>(90/B13) * E13</f>
+        <f t="shared" si="3"/>
         <v>0.5787781350482315</v>
       </c>
     </row>
@@ -944,19 +948,19 @@
         <v>2</v>
       </c>
       <c r="E14">
-        <f>C14+D14</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F14">
-        <f xml:space="preserve"> (90 / B14) * C14</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G14">
-        <f>(90/B14)*D14</f>
+        <f t="shared" si="2"/>
         <v>0.55214723926380371</v>
       </c>
       <c r="H14">
-        <f>(90/B14) * E14</f>
+        <f t="shared" si="3"/>
         <v>0.55214723926380371</v>
       </c>
     </row>
@@ -974,19 +978,19 @@
         <v>2</v>
       </c>
       <c r="E15">
-        <f>C15+D15</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F15">
-        <f xml:space="preserve"> (90 / B15) * C15</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G15">
-        <f>(90/B15)*D15</f>
+        <f t="shared" si="2"/>
         <v>0.53892215568862278</v>
       </c>
       <c r="H15">
-        <f>(90/B15) * E15</f>
+        <f t="shared" si="3"/>
         <v>0.53892215568862278</v>
       </c>
     </row>
@@ -1004,19 +1008,19 @@
         <v>1</v>
       </c>
       <c r="E16">
-        <f>C16+D16</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="F16">
-        <f xml:space="preserve"> (90 / B16) * C16</f>
+        <f t="shared" si="1"/>
         <v>0.34682080924855491</v>
       </c>
       <c r="G16">
-        <f>(90/B16)*D16</f>
+        <f t="shared" si="2"/>
         <v>0.17341040462427745</v>
       </c>
       <c r="H16">
-        <f>(90/B16) * E16</f>
+        <f t="shared" si="3"/>
         <v>0.52023121387283233</v>
       </c>
     </row>
@@ -1034,19 +1038,19 @@
         <v>2</v>
       </c>
       <c r="E17">
-        <f>C17+D17</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F17">
-        <f xml:space="preserve"> (90 / B17) * C17</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G17">
-        <f>(90/B17)*D17</f>
+        <f t="shared" si="2"/>
         <v>0.46753246753246752</v>
       </c>
       <c r="H17">
-        <f>(90/B17) * E17</f>
+        <f t="shared" si="3"/>
         <v>0.46753246753246752</v>
       </c>
     </row>
@@ -1064,19 +1068,19 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <f>C18+D18</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F18">
-        <f xml:space="preserve"> (90 / B18) * C18</f>
+        <f t="shared" si="1"/>
         <v>0.41095890410958902</v>
       </c>
       <c r="G18">
-        <f>(90/B18)*D18</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H18">
-        <f>(90/B18) * E18</f>
+        <f t="shared" si="3"/>
         <v>0.41095890410958902</v>
       </c>
     </row>
@@ -1094,19 +1098,19 @@
         <v>1</v>
       </c>
       <c r="E19">
-        <f>C19+D19</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F19">
-        <f xml:space="preserve"> (90 / B19) * C19</f>
+        <f t="shared" si="1"/>
         <v>0.19438444924406048</v>
       </c>
       <c r="G19">
-        <f>(90/B19)*D19</f>
+        <f t="shared" si="2"/>
         <v>0.19438444924406048</v>
       </c>
       <c r="H19">
-        <f>(90/B19) * E19</f>
+        <f t="shared" si="3"/>
         <v>0.38876889848812096</v>
       </c>
     </row>
@@ -1126,7 +1130,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1170,7 +1174,7 @@
         <v>141</v>
       </c>
       <c r="D2">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>13</v>
@@ -1190,7 +1194,7 @@
         <v>16</v>
       </c>
       <c r="D3">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>14</v>
@@ -1210,7 +1214,7 @@
         <v>35</v>
       </c>
       <c r="D4">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>14</v>
@@ -1230,7 +1234,7 @@
         <v>8</v>
       </c>
       <c r="D5">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>14</v>
@@ -1250,7 +1254,7 @@
         <v>70</v>
       </c>
       <c r="D6">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>14</v>
@@ -1270,7 +1274,7 @@
         <v>136</v>
       </c>
       <c r="D7">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>13</v>
@@ -1290,7 +1294,7 @@
         <v>34</v>
       </c>
       <c r="D8">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>14</v>
@@ -1310,7 +1314,7 @@
         <v>27</v>
       </c>
       <c r="D9">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>14</v>
@@ -1330,7 +1334,7 @@
         <v>32</v>
       </c>
       <c r="D10">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>14</v>
@@ -1350,7 +1354,7 @@
         <v>7</v>
       </c>
       <c r="D11">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>14</v>
@@ -1370,7 +1374,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1413,7 +1417,7 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>14</v>
@@ -1433,7 +1437,7 @@
         <v>146</v>
       </c>
       <c r="D3">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>13</v>
@@ -1453,7 +1457,7 @@
         <v>8</v>
       </c>
       <c r="D4">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>14</v>
@@ -1473,7 +1477,7 @@
         <v>12</v>
       </c>
       <c r="D5">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>14</v>
@@ -1513,7 +1517,7 @@
         <v>37</v>
       </c>
       <c r="D7">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>14</v>
@@ -1533,7 +1537,7 @@
         <v>29</v>
       </c>
       <c r="D8">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>13</v>
@@ -1553,7 +1557,7 @@
         <v>136</v>
       </c>
       <c r="D9">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>13</v>
@@ -1573,7 +1577,7 @@
         <v>7</v>
       </c>
       <c r="D10">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>14</v>
@@ -1593,7 +1597,7 @@
         <v>10</v>
       </c>
       <c r="D11">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>14</v>
@@ -1613,7 +1617,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1655,7 +1659,7 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>14</v>
@@ -1675,7 +1679,7 @@
         <v>8</v>
       </c>
       <c r="D3">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>14</v>
@@ -1695,7 +1699,7 @@
         <v>141</v>
       </c>
       <c r="D4">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
@@ -1715,7 +1719,7 @@
         <v>136</v>
       </c>
       <c r="D5">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>13</v>
@@ -1735,7 +1739,7 @@
         <v>16</v>
       </c>
       <c r="D6">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>14</v>
@@ -1755,7 +1759,7 @@
         <v>35</v>
       </c>
       <c r="D7">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>14</v>
@@ -1775,7 +1779,7 @@
         <v>146</v>
       </c>
       <c r="D8">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>13</v>
@@ -1795,7 +1799,7 @@
         <v>70</v>
       </c>
       <c r="D9">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>14</v>
@@ -1815,7 +1819,7 @@
         <v>34</v>
       </c>
       <c r="D10">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>14</v>
@@ -1835,7 +1839,7 @@
         <v>12</v>
       </c>
       <c r="D11">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Rerun vaep ranking generator for specific type ids only
</commit_message>
<xml_diff>
--- a/notebooks/data/players_skill_dataset/Transfermarkt Euro 2020 Comparison.xlsx
+++ b/notebooks/data/players_skill_dataset/Transfermarkt Euro 2020 Comparison.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://itbdsti-my.sharepoint.com/personal/23522016_mahasiswa_itb_ac_id/Documents/Informatika S2/Semester 3/IF6099 Thesis/Draft Thesis/Thesis/Source Code/vaep-base-code/notebooks/data/players_skill_dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="605" documentId="11_F25DC773A252ABDACC104849C99C61665BDE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D13A325E-BD36-41B6-82CF-0FD0A2754DCE}"/>
+  <xr:revisionPtr revIDLastSave="729" documentId="11_F25DC773A252ABDACC104849C99C61665BDE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E566A37F-A136-4EBC-A5E8-151632637829}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basis" sheetId="1" r:id="rId1"/>
     <sheet name="Top 10 players goal 90" sheetId="2" r:id="rId2"/>
     <sheet name="Top 10 players assist 90" sheetId="3" r:id="rId3"/>
     <sheet name="Top 10 players goal assist 90" sheetId="4" r:id="rId4"/>
+    <sheet name="Top 10 VAEP ranking" sheetId="5" r:id="rId5"/>
+    <sheet name="Top 10 proposed ranking" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Basis!$A$1:$H$1</definedName>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="80">
   <si>
     <t>Player Name</t>
   </si>
@@ -186,6 +188,102 @@
   </si>
   <si>
     <t>1.6 million euro</t>
+  </si>
+  <si>
+    <t>Ranking VAEP</t>
+  </si>
+  <si>
+    <t>Ranking Proposed</t>
+  </si>
+  <si>
+    <t>Steven Berghuis</t>
+  </si>
+  <si>
+    <t>Timo Werner</t>
+  </si>
+  <si>
+    <t>Enis Bardhi</t>
+  </si>
+  <si>
+    <t>Kingsley Coman</t>
+  </si>
+  <si>
+    <t>Kevin Varga</t>
+  </si>
+  <si>
+    <t>Bruno Fernandes</t>
+  </si>
+  <si>
+    <t>Eric Garcia</t>
+  </si>
+  <si>
+    <t>15 million euro</t>
+  </si>
+  <si>
+    <t>42 million euro</t>
+  </si>
+  <si>
+    <t>8 million euro</t>
+  </si>
+  <si>
+    <t>Stuart Armstrong</t>
+  </si>
+  <si>
+    <t>6 million euro</t>
+  </si>
+  <si>
+    <t>0,5 million euro</t>
+  </si>
+  <si>
+    <t>60 million euro</t>
+  </si>
+  <si>
+    <t>2,1 million euro</t>
+  </si>
+  <si>
+    <t>18 million euro</t>
+  </si>
+  <si>
+    <t>Patrik Hrosovsky</t>
+  </si>
+  <si>
+    <t>Laszlo Benes</t>
+  </si>
+  <si>
+    <t>Ousmane Dembele</t>
+  </si>
+  <si>
+    <t>Dominic Calvert-Lewin</t>
+  </si>
+  <si>
+    <t>Sergio Busquets</t>
+  </si>
+  <si>
+    <t>Thiago Alcantara</t>
+  </si>
+  <si>
+    <t>Cesar Azpilicueta</t>
+  </si>
+  <si>
+    <t>Sime Vrsaljko</t>
+  </si>
+  <si>
+    <t>5 million euro</t>
+  </si>
+  <si>
+    <t>70 million euro</t>
+  </si>
+  <si>
+    <t>30 million euro</t>
+  </si>
+  <si>
+    <t>28 million euro</t>
+  </si>
+  <si>
+    <t>284,6 million euro</t>
+  </si>
+  <si>
+    <t>275 million euro</t>
   </si>
 </sst>
 </file>
@@ -1128,9 +1226,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65E8B2B0-9B16-4C07-8D13-5F3B45B2B4EF}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1171,7 +1269,7 @@
         <v>1.267605633802817</v>
       </c>
       <c r="C2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D2">
         <v>77</v>
@@ -1191,7 +1289,7 @@
         <v>0.96256684491978606</v>
       </c>
       <c r="C3">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <v>102</v>
@@ -1211,7 +1309,7 @@
         <v>0.87662337662337664</v>
       </c>
       <c r="C4">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D4">
         <v>108</v>
@@ -1231,7 +1329,7 @@
         <v>0.74380165289256195</v>
       </c>
       <c r="C5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>49</v>
@@ -1251,7 +1349,7 @@
         <v>0.69498069498069504</v>
       </c>
       <c r="C6">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D6">
         <v>89</v>
@@ -1271,13 +1369,13 @@
         <v>0.66420664206642066</v>
       </c>
       <c r="C7">
-        <v>136</v>
+        <v>33</v>
       </c>
       <c r="D7">
         <v>58</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>37</v>
@@ -1291,7 +1389,7 @@
         <v>0.4580152671755725</v>
       </c>
       <c r="C8">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D8">
         <v>103</v>
@@ -1311,7 +1409,7 @@
         <v>0.41095890410958902</v>
       </c>
       <c r="C9">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D9">
         <v>43</v>
@@ -1331,7 +1429,7 @@
         <v>0.34682080924855491</v>
       </c>
       <c r="C10">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D10">
         <v>54</v>
@@ -1351,7 +1449,7 @@
         <v>0.29411764705882354</v>
       </c>
       <c r="C11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D11">
         <v>20</v>
@@ -1374,7 +1472,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1414,13 +1512,13 @@
         <v>4.3902439024390247</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="D2">
         <v>6</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>42</v>
@@ -1434,7 +1532,7 @@
         <v>0.8</v>
       </c>
       <c r="C3">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D3">
         <v>35</v>
@@ -1454,7 +1552,7 @@
         <v>0.74380165289256195</v>
       </c>
       <c r="C4">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>49</v>
@@ -1474,7 +1572,7 @@
         <v>0.62937062937062938</v>
       </c>
       <c r="C5">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <v>29</v>
@@ -1494,7 +1592,7 @@
         <v>0.55214723926380371</v>
       </c>
       <c r="C6">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D6">
         <v>74</v>
@@ -1514,13 +1612,13 @@
         <v>0.53892215568862278</v>
       </c>
       <c r="C7">
-        <v>37</v>
+        <v>139</v>
       </c>
       <c r="D7">
         <v>85</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>46</v>
@@ -1534,13 +1632,13 @@
         <v>0.46753246753246752</v>
       </c>
       <c r="C8">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D8">
         <v>27</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>47</v>
@@ -1554,13 +1652,13 @@
         <v>0.33210332103321033</v>
       </c>
       <c r="C9">
-        <v>136</v>
+        <v>33</v>
       </c>
       <c r="D9">
         <v>58</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>37</v>
@@ -1574,7 +1672,7 @@
         <v>0.29411764705882354</v>
       </c>
       <c r="C10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10">
         <v>20</v>
@@ -1594,7 +1692,7 @@
         <v>0.28938906752411575</v>
       </c>
       <c r="C11">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D11">
         <v>59</v>
@@ -1615,9 +1713,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3646684C-3C25-4047-A473-E5B86158F854}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1656,13 +1754,13 @@
         <v>4.3902439024390247</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="D2">
         <v>6</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>42</v>
@@ -1676,7 +1774,7 @@
         <v>1.4876033057851239</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>49</v>
@@ -1696,7 +1794,7 @@
         <v>1.267605633802817</v>
       </c>
       <c r="C4">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D4">
         <v>77</v>
@@ -1716,7 +1814,7 @@
         <v>0.99630996309963105</v>
       </c>
       <c r="C5">
-        <v>136</v>
+        <v>33</v>
       </c>
       <c r="D5">
         <v>58</v>
@@ -1736,7 +1834,7 @@
         <v>0.96256684491978606</v>
       </c>
       <c r="C6">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <v>102</v>
@@ -1756,7 +1854,7 @@
         <v>0.87662337662337664</v>
       </c>
       <c r="C7">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D7">
         <v>108</v>
@@ -1776,7 +1874,7 @@
         <v>0.8</v>
       </c>
       <c r="C8">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D8">
         <v>35</v>
@@ -1796,7 +1894,7 @@
         <v>0.69498069498069504</v>
       </c>
       <c r="C9">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D9">
         <v>89</v>
@@ -1816,7 +1914,7 @@
         <v>0.68702290076335881</v>
       </c>
       <c r="C10">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D10">
         <v>103</v>
@@ -1836,7 +1934,7 @@
         <v>0.62937062937062938</v>
       </c>
       <c r="C11">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D11">
         <v>29</v>
@@ -1846,6 +1944,300 @@
       </c>
       <c r="F11" s="3" t="s">
         <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32BF042F-4DC6-4D26-80FC-472AD3B46905}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.26953125" customWidth="1"/>
+    <col min="2" max="2" width="19.08984375" customWidth="1"/>
+    <col min="3" max="3" width="18.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B41235B2-BFDE-488F-B400-69087D6E62FC}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" width="20.54296875" customWidth="1"/>
+    <col min="3" max="3" width="19.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update latest euro player potential
</commit_message>
<xml_diff>
--- a/notebooks/data/players_skill_dataset/Transfermarkt Euro 2020 Comparison.xlsx
+++ b/notebooks/data/players_skill_dataset/Transfermarkt Euro 2020 Comparison.xlsx
@@ -1226,9 +1226,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65E8B2B0-9B16-4C07-8D13-5F3B45B2B4EF}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1472,7 +1472,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1715,7 +1715,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1957,7 +1957,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2104,7 +2104,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Run experiment for vaep ranking and proposed ranking
</commit_message>
<xml_diff>
--- a/notebooks/data/players_skill_dataset/Transfermarkt Euro 2020 Comparison.xlsx
+++ b/notebooks/data/players_skill_dataset/Transfermarkt Euro 2020 Comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://itbdsti-my.sharepoint.com/personal/23522016_mahasiswa_itb_ac_id/Documents/Informatika S2/Semester 3/IF6099 Thesis/Draft Thesis/Thesis/Source Code/vaep-base-code/notebooks/data/players_skill_dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="729" documentId="11_F25DC773A252ABDACC104849C99C61665BDE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E566A37F-A136-4EBC-A5E8-151632637829}"/>
+  <xr:revisionPtr revIDLastSave="834" documentId="11_F25DC773A252ABDACC104849C99C61665BDE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9A4FC24-2F50-4D00-B0A1-181F21D40F20}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="81">
   <si>
     <t>Player Name</t>
   </si>
@@ -199,91 +199,94 @@
     <t>Steven Berghuis</t>
   </si>
   <si>
-    <t>Timo Werner</t>
-  </si>
-  <si>
-    <t>Enis Bardhi</t>
-  </si>
-  <si>
     <t>Kingsley Coman</t>
   </si>
   <si>
     <t>Kevin Varga</t>
   </si>
   <si>
-    <t>Bruno Fernandes</t>
-  </si>
-  <si>
     <t>Eric Garcia</t>
   </si>
   <si>
-    <t>15 million euro</t>
-  </si>
-  <si>
-    <t>42 million euro</t>
-  </si>
-  <si>
     <t>8 million euro</t>
   </si>
   <si>
-    <t>Stuart Armstrong</t>
-  </si>
-  <si>
-    <t>6 million euro</t>
-  </si>
-  <si>
-    <t>0,5 million euro</t>
-  </si>
-  <si>
-    <t>60 million euro</t>
-  </si>
-  <si>
-    <t>2,1 million euro</t>
-  </si>
-  <si>
-    <t>18 million euro</t>
-  </si>
-  <si>
-    <t>Patrik Hrosovsky</t>
-  </si>
-  <si>
     <t>Laszlo Benes</t>
   </si>
   <si>
     <t>Ousmane Dembele</t>
   </si>
   <si>
-    <t>Dominic Calvert-Lewin</t>
-  </si>
-  <si>
-    <t>Sergio Busquets</t>
-  </si>
-  <si>
-    <t>Thiago Alcantara</t>
-  </si>
-  <si>
-    <t>Cesar Azpilicueta</t>
-  </si>
-  <si>
-    <t>Sime Vrsaljko</t>
-  </si>
-  <si>
     <t>5 million euro</t>
   </si>
   <si>
     <t>70 million euro</t>
   </si>
   <si>
-    <t>30 million euro</t>
-  </si>
-  <si>
     <t>28 million euro</t>
   </si>
   <si>
-    <t>284,6 million euro</t>
-  </si>
-  <si>
-    <t>275 million euro</t>
+    <t>Joao Palhinha</t>
+  </si>
+  <si>
+    <t>Karol Linetty</t>
+  </si>
+  <si>
+    <t>Harry Wilson</t>
+  </si>
+  <si>
+    <t>Sasa Kalajdzic</t>
+  </si>
+  <si>
+    <t>Luke Armstrong</t>
+  </si>
+  <si>
+    <t>Patrik Hrozovsky</t>
+  </si>
+  <si>
+    <t>Matthias Ginter</t>
+  </si>
+  <si>
+    <t>Ilkay Gundogan</t>
+  </si>
+  <si>
+    <t>William Carvalho</t>
+  </si>
+  <si>
+    <t>0,55 million euro</t>
+  </si>
+  <si>
+    <t>4,8 million euro</t>
+  </si>
+  <si>
+    <t>11 million euro</t>
+  </si>
+  <si>
+    <t>22 million euro</t>
+  </si>
+  <si>
+    <t>Przemyslaw Frankowski</t>
+  </si>
+  <si>
+    <t>1,6 million euro</t>
+  </si>
+  <si>
+    <t>0,15 million euro</t>
+  </si>
+  <si>
+    <t>135,1 million euro</t>
+  </si>
+  <si>
+    <t>6,3 million euro</t>
+  </si>
+  <si>
+    <t>14 million euro</t>
+  </si>
+  <si>
+    <t>40 million euro</t>
+  </si>
+  <si>
+    <t>242,3 million euro</t>
   </si>
 </sst>
 </file>
@@ -1228,7 +1231,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:D11"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1269,10 +1272,10 @@
         <v>1.267605633802817</v>
       </c>
       <c r="C2">
-        <v>142</v>
+        <v>105</v>
       </c>
       <c r="D2">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>13</v>
@@ -1289,10 +1292,10 @@
         <v>0.96256684491978606</v>
       </c>
       <c r="C3">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D3">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>14</v>
@@ -1309,10 +1312,10 @@
         <v>0.87662337662337664</v>
       </c>
       <c r="C4">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="D4">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>14</v>
@@ -1329,10 +1332,10 @@
         <v>0.74380165289256195</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>89</v>
       </c>
       <c r="D5">
-        <v>49</v>
+        <v>100</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>14</v>
@@ -1349,10 +1352,10 @@
         <v>0.69498069498069504</v>
       </c>
       <c r="C6">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="D6">
-        <v>89</v>
+        <v>112</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>14</v>
@@ -1369,10 +1372,10 @@
         <v>0.66420664206642066</v>
       </c>
       <c r="C7">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D7">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>14</v>
@@ -1389,10 +1392,10 @@
         <v>0.4580152671755725</v>
       </c>
       <c r="C8">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="D8">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>14</v>
@@ -1409,10 +1412,10 @@
         <v>0.41095890410958902</v>
       </c>
       <c r="C9">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D9">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>14</v>
@@ -1429,10 +1432,10 @@
         <v>0.34682080924855491</v>
       </c>
       <c r="C10">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="D10">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>14</v>
@@ -1449,13 +1452,13 @@
         <v>0.29411764705882354</v>
       </c>
       <c r="C11">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="D11">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>41</v>
@@ -1472,7 +1475,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:D11"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1512,13 +1515,13 @@
         <v>4.3902439024390247</v>
       </c>
       <c r="C2">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>42</v>
@@ -1532,10 +1535,10 @@
         <v>0.8</v>
       </c>
       <c r="C3">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D3">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>13</v>
@@ -1552,10 +1555,10 @@
         <v>0.74380165289256195</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>89</v>
       </c>
       <c r="D4">
-        <v>49</v>
+        <v>100</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>14</v>
@@ -1572,13 +1575,13 @@
         <v>0.62937062937062938</v>
       </c>
       <c r="C5">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="D5">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>44</v>
@@ -1592,13 +1595,13 @@
         <v>0.55214723926380371</v>
       </c>
       <c r="C6">
-        <v>146</v>
+        <v>80</v>
       </c>
       <c r="D6">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>45</v>
@@ -1612,10 +1615,10 @@
         <v>0.53892215568862278</v>
       </c>
       <c r="C7">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="D7">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>13</v>
@@ -1632,10 +1635,10 @@
         <v>0.46753246753246752</v>
       </c>
       <c r="C8">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="D8">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>14</v>
@@ -1652,10 +1655,10 @@
         <v>0.33210332103321033</v>
       </c>
       <c r="C9">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D9">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>14</v>
@@ -1672,13 +1675,13 @@
         <v>0.29411764705882354</v>
       </c>
       <c r="C10">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="D10">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>41</v>
@@ -1692,10 +1695,10 @@
         <v>0.28938906752411575</v>
       </c>
       <c r="C11">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D11">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>14</v>
@@ -1715,7 +1718,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:D11"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1754,13 +1757,13 @@
         <v>4.3902439024390247</v>
       </c>
       <c r="C2">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>42</v>
@@ -1774,10 +1777,10 @@
         <v>1.4876033057851239</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>89</v>
       </c>
       <c r="D3">
-        <v>49</v>
+        <v>100</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>14</v>
@@ -1794,10 +1797,10 @@
         <v>1.267605633802817</v>
       </c>
       <c r="C4">
-        <v>142</v>
+        <v>105</v>
       </c>
       <c r="D4">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
@@ -1814,10 +1817,10 @@
         <v>0.99630996309963105</v>
       </c>
       <c r="C5">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D5">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>13</v>
@@ -1834,10 +1837,10 @@
         <v>0.96256684491978606</v>
       </c>
       <c r="C6">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D6">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>14</v>
@@ -1854,10 +1857,10 @@
         <v>0.87662337662337664</v>
       </c>
       <c r="C7">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="D7">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>14</v>
@@ -1874,10 +1877,10 @@
         <v>0.8</v>
       </c>
       <c r="C8">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D8">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>13</v>
@@ -1894,10 +1897,10 @@
         <v>0.69498069498069504</v>
       </c>
       <c r="C9">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="D9">
-        <v>89</v>
+        <v>112</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>14</v>
@@ -1914,10 +1917,10 @@
         <v>0.68702290076335881</v>
       </c>
       <c r="C10">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="D10">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>14</v>
@@ -1934,13 +1937,13 @@
         <v>0.62937062937062938</v>
       </c>
       <c r="C11">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="D11">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>44</v>
@@ -1957,13 +1960,13 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B11"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.26953125" customWidth="1"/>
-    <col min="2" max="2" width="19.08984375" customWidth="1"/>
+    <col min="2" max="2" width="21.1796875" customWidth="1"/>
     <col min="3" max="3" width="18.08984375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1983,10 +1986,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1994,10 +1997,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -2005,10 +2008,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -2019,7 +2022,7 @@
         <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -2027,10 +2030,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -2038,10 +2041,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -2049,10 +2052,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -2060,10 +2063,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -2071,10 +2074,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -2082,15 +2085,15 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2104,7 +2107,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B11"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2130,10 +2133,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -2141,10 +2144,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -2152,10 +2155,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -2163,10 +2166,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -2174,10 +2177,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -2185,10 +2188,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -2196,10 +2199,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -2207,10 +2210,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -2218,10 +2221,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -2229,15 +2232,15 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rerun all experiment using PR curve method to find threshold
</commit_message>
<xml_diff>
--- a/notebooks/data/players_skill_dataset/Transfermarkt Euro 2020 Comparison.xlsx
+++ b/notebooks/data/players_skill_dataset/Transfermarkt Euro 2020 Comparison.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://itbdsti-my.sharepoint.com/personal/23522016_mahasiswa_itb_ac_id/Documents/Informatika S2/Semester 3/IF6099 Thesis/Draft Thesis/Thesis/Source Code/vaep-base-code/notebooks/data/players_skill_dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="834" documentId="11_F25DC773A252ABDACC104849C99C61665BDE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9A4FC24-2F50-4D00-B0A1-181F21D40F20}"/>
+  <xr:revisionPtr revIDLastSave="876" documentId="11_F25DC773A252ABDACC104849C99C61665BDE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56F3D7D1-61D4-4961-AAEE-2EE7E0B6F601}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="82">
   <si>
     <t>Player Name</t>
   </si>
@@ -286,7 +286,10 @@
     <t>40 million euro</t>
   </si>
   <si>
-    <t>242,3 million euro</t>
+    <t>Thiago Alcantara</t>
+  </si>
+  <si>
+    <t>255,3 million euro</t>
   </si>
 </sst>
 </file>
@@ -1231,7 +1234,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8:D8"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1355,7 +1358,7 @@
         <v>74</v>
       </c>
       <c r="D6">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>14</v>
@@ -1455,7 +1458,7 @@
         <v>58</v>
       </c>
       <c r="D11">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>13</v>
@@ -1475,7 +1478,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5:D5"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1518,7 +1521,7 @@
         <v>3</v>
       </c>
       <c r="D2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>14</v>
@@ -1598,7 +1601,7 @@
         <v>80</v>
       </c>
       <c r="D6">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>14</v>
@@ -1638,7 +1641,7 @@
         <v>41</v>
       </c>
       <c r="D8">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>14</v>
@@ -1678,7 +1681,7 @@
         <v>58</v>
       </c>
       <c r="D10">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>13</v>
@@ -1698,7 +1701,7 @@
         <v>26</v>
       </c>
       <c r="D11">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>14</v>
@@ -1718,7 +1721,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1760,7 +1763,7 @@
         <v>3</v>
       </c>
       <c r="D2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>14</v>
@@ -1823,7 +1826,7 @@
         <v>72</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>37</v>
@@ -1900,7 +1903,7 @@
         <v>74</v>
       </c>
       <c r="D9">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>14</v>
@@ -2107,7 +2110,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2199,10 +2202,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -2221,10 +2224,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -2232,15 +2235,15 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rerun experiment for accuracy threshold only
</commit_message>
<xml_diff>
--- a/notebooks/data/players_skill_dataset/Transfermarkt Euro 2020 Comparison.xlsx
+++ b/notebooks/data/players_skill_dataset/Transfermarkt Euro 2020 Comparison.xlsx
@@ -1234,7 +1234,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1478,7 +1478,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1721,7 +1721,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1963,7 +1963,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2110,7 +2110,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Rerun all experiment (use fully train data to determine threshold)
</commit_message>
<xml_diff>
--- a/notebooks/data/players_skill_dataset/Transfermarkt Euro 2020 Comparison.xlsx
+++ b/notebooks/data/players_skill_dataset/Transfermarkt Euro 2020 Comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://itbdsti-my.sharepoint.com/personal/23522016_mahasiswa_itb_ac_id/Documents/Informatika S2/Semester 3/IF6099 Thesis/Draft Thesis/Thesis/Source Code/vaep-base-code/notebooks/data/players_skill_dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="876" documentId="11_F25DC773A252ABDACC104849C99C61665BDE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56F3D7D1-61D4-4961-AAEE-2EE7E0B6F601}"/>
+  <xr:revisionPtr revIDLastSave="921" documentId="11_F25DC773A252ABDACC104849C99C61665BDE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DD89CF1-D406-4103-9607-BE47ACD3896C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="81">
   <si>
     <t>Player Name</t>
   </si>
@@ -223,9 +223,6 @@
     <t>70 million euro</t>
   </si>
   <si>
-    <t>28 million euro</t>
-  </si>
-  <si>
     <t>Joao Palhinha</t>
   </si>
   <si>
@@ -244,9 +241,6 @@
     <t>Patrik Hrozovsky</t>
   </si>
   <si>
-    <t>Matthias Ginter</t>
-  </si>
-  <si>
     <t>Ilkay Gundogan</t>
   </si>
   <si>
@@ -286,10 +280,13 @@
     <t>40 million euro</t>
   </si>
   <si>
-    <t>Thiago Alcantara</t>
-  </si>
-  <si>
-    <t>255,3 million euro</t>
+    <t>Quincy Promes</t>
+  </si>
+  <si>
+    <t>17.5 million euro</t>
+  </si>
+  <si>
+    <t>231,8 million euro</t>
   </si>
 </sst>
 </file>
@@ -1234,7 +1231,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:D11"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1278,7 +1275,7 @@
         <v>105</v>
       </c>
       <c r="D2">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>13</v>
@@ -1298,7 +1295,7 @@
         <v>40</v>
       </c>
       <c r="D3">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>14</v>
@@ -1318,7 +1315,7 @@
         <v>82</v>
       </c>
       <c r="D4">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>14</v>
@@ -1358,7 +1355,7 @@
         <v>74</v>
       </c>
       <c r="D6">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>14</v>
@@ -1378,7 +1375,7 @@
         <v>44</v>
       </c>
       <c r="D7">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>14</v>
@@ -1398,7 +1395,7 @@
         <v>48</v>
       </c>
       <c r="D8">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>14</v>
@@ -1418,7 +1415,7 @@
         <v>36</v>
       </c>
       <c r="D9">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>14</v>
@@ -1438,7 +1435,7 @@
         <v>49</v>
       </c>
       <c r="D10">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>14</v>
@@ -1458,7 +1455,7 @@
         <v>58</v>
       </c>
       <c r="D11">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>13</v>
@@ -1478,7 +1475,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:D11"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1521,7 +1518,7 @@
         <v>3</v>
       </c>
       <c r="D2">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>14</v>
@@ -1541,7 +1538,7 @@
         <v>146</v>
       </c>
       <c r="D3">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>13</v>
@@ -1601,7 +1598,7 @@
         <v>80</v>
       </c>
       <c r="D6">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>14</v>
@@ -1621,7 +1618,7 @@
         <v>145</v>
       </c>
       <c r="D7">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>13</v>
@@ -1641,7 +1638,7 @@
         <v>41</v>
       </c>
       <c r="D8">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>14</v>
@@ -1661,7 +1658,7 @@
         <v>44</v>
       </c>
       <c r="D9">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>14</v>
@@ -1681,7 +1678,7 @@
         <v>58</v>
       </c>
       <c r="D10">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>13</v>
@@ -1701,10 +1698,10 @@
         <v>26</v>
       </c>
       <c r="D11">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>33</v>
@@ -1721,7 +1718,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:D11"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1763,7 +1760,7 @@
         <v>3</v>
       </c>
       <c r="D2">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>14</v>
@@ -1803,7 +1800,7 @@
         <v>105</v>
       </c>
       <c r="D4">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
@@ -1823,7 +1820,7 @@
         <v>44</v>
       </c>
       <c r="D5">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>14</v>
@@ -1843,7 +1840,7 @@
         <v>40</v>
       </c>
       <c r="D6">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>14</v>
@@ -1863,7 +1860,7 @@
         <v>82</v>
       </c>
       <c r="D7">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>14</v>
@@ -1883,7 +1880,7 @@
         <v>146</v>
       </c>
       <c r="D8">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>13</v>
@@ -1903,7 +1900,7 @@
         <v>74</v>
       </c>
       <c r="D9">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>14</v>
@@ -1923,7 +1920,7 @@
         <v>48</v>
       </c>
       <c r="D10">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>14</v>
@@ -1963,7 +1960,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B11"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1992,7 +1989,7 @@
         <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -2022,10 +2019,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -2033,10 +2030,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -2044,10 +2041,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -2066,10 +2063,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -2077,7 +2074,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
         <v>32</v>
@@ -2088,15 +2085,15 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2110,7 +2107,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B11"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2118,6 +2115,7 @@
     <col min="1" max="1" width="18.54296875" customWidth="1"/>
     <col min="2" max="2" width="20.54296875" customWidth="1"/>
     <col min="3" max="3" width="19.90625" customWidth="1"/>
+    <col min="5" max="5" width="17.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -2136,7 +2134,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>57</v>
@@ -2172,7 +2170,7 @@
         <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -2183,7 +2181,7 @@
         <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -2202,10 +2200,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -2213,10 +2211,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -2224,10 +2222,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -2235,15 +2233,15 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rerun all experiment : convert linear regression to logistic regression
</commit_message>
<xml_diff>
--- a/notebooks/data/players_skill_dataset/Transfermarkt Euro 2020 Comparison.xlsx
+++ b/notebooks/data/players_skill_dataset/Transfermarkt Euro 2020 Comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://itbdsti-my.sharepoint.com/personal/23522016_mahasiswa_itb_ac_id/Documents/Informatika S2/Semester 3/IF6099 Thesis/Draft Thesis/Thesis/Source Code/vaep-base-code/notebooks/data/players_skill_dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="921" documentId="11_F25DC773A252ABDACC104849C99C61665BDE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DD89CF1-D406-4103-9607-BE47ACD3896C}"/>
+  <xr:revisionPtr revIDLastSave="965" documentId="11_F25DC773A252ABDACC104849C99C61665BDE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AD69292-9B26-472F-A292-D0F27AB4B0B4}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -280,13 +280,13 @@
     <t>40 million euro</t>
   </si>
   <si>
-    <t>Quincy Promes</t>
-  </si>
-  <si>
-    <t>17.5 million euro</t>
-  </si>
-  <si>
-    <t>231,8 million euro</t>
+    <t>Matthias Ginter</t>
+  </si>
+  <si>
+    <t>28 million euro</t>
+  </si>
+  <si>
+    <t>242,3 million euro</t>
   </si>
 </sst>
 </file>
@@ -1275,7 +1275,7 @@
         <v>105</v>
       </c>
       <c r="D2">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>13</v>
@@ -1295,7 +1295,7 @@
         <v>40</v>
       </c>
       <c r="D3">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>14</v>
@@ -1335,7 +1335,7 @@
         <v>89</v>
       </c>
       <c r="D5">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>14</v>
@@ -1375,7 +1375,7 @@
         <v>44</v>
       </c>
       <c r="D7">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>14</v>
@@ -1395,7 +1395,7 @@
         <v>48</v>
       </c>
       <c r="D8">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>14</v>
@@ -1415,7 +1415,7 @@
         <v>36</v>
       </c>
       <c r="D9">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>14</v>
@@ -1435,7 +1435,7 @@
         <v>49</v>
       </c>
       <c r="D10">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>14</v>
@@ -1455,7 +1455,7 @@
         <v>58</v>
       </c>
       <c r="D11">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>13</v>
@@ -1475,7 +1475,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D11"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1518,7 +1518,7 @@
         <v>3</v>
       </c>
       <c r="D2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>14</v>
@@ -1538,7 +1538,7 @@
         <v>146</v>
       </c>
       <c r="D3">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>13</v>
@@ -1558,7 +1558,7 @@
         <v>89</v>
       </c>
       <c r="D4">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>14</v>
@@ -1578,7 +1578,7 @@
         <v>38</v>
       </c>
       <c r="D5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>13</v>
@@ -1598,7 +1598,7 @@
         <v>80</v>
       </c>
       <c r="D6">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>14</v>
@@ -1618,7 +1618,7 @@
         <v>145</v>
       </c>
       <c r="D7">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>13</v>
@@ -1638,7 +1638,7 @@
         <v>41</v>
       </c>
       <c r="D8">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>14</v>
@@ -1658,7 +1658,7 @@
         <v>44</v>
       </c>
       <c r="D9">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>14</v>
@@ -1678,7 +1678,7 @@
         <v>58</v>
       </c>
       <c r="D10">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>13</v>
@@ -1698,10 +1698,10 @@
         <v>26</v>
       </c>
       <c r="D11">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>33</v>
@@ -1760,7 +1760,7 @@
         <v>3</v>
       </c>
       <c r="D2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>14</v>
@@ -1780,7 +1780,7 @@
         <v>89</v>
       </c>
       <c r="D3">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>14</v>
@@ -1800,7 +1800,7 @@
         <v>105</v>
       </c>
       <c r="D4">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
@@ -1820,7 +1820,7 @@
         <v>44</v>
       </c>
       <c r="D5">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>14</v>
@@ -1840,7 +1840,7 @@
         <v>40</v>
       </c>
       <c r="D6">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>14</v>
@@ -1880,7 +1880,7 @@
         <v>146</v>
       </c>
       <c r="D8">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>13</v>
@@ -1920,7 +1920,7 @@
         <v>48</v>
       </c>
       <c r="D10">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>14</v>
@@ -1940,7 +1940,7 @@
         <v>38</v>
       </c>
       <c r="D11">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>13</v>
@@ -1960,7 +1960,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2107,7 +2107,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2178,10 +2178,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -2189,10 +2189,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -2200,10 +2200,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -2222,10 +2222,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -2233,10 +2233,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>